<commit_message>
Commit with updated variable list
</commit_message>
<xml_diff>
--- a/elsa/G2A ELSA Longitudinal Variable List.xlsx
+++ b/elsa/G2A ELSA Longitudinal Variable List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8690691-A70A-4353-A5AB-BE57CAADD43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB9270F-6D45-4725-BB2C-0A3CB76940D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-15840" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-14520" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="biomarkers" sheetId="9" r:id="rId1"/>
@@ -2730,7 +2730,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>